<commit_message>
changed according to teacher
</commit_message>
<xml_diff>
--- a/Sprint Sheet.xlsx
+++ b/Sprint Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SIlencedFrost\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thnrg\Documents\Nhap Mon KT Phan Mem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65960A55-967A-4E36-B25D-ED667C8FB5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE6BA9-D238-4E3D-83D0-0FEB86041FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="2895" windowWidth="21600" windowHeight="11175" xr2:uid="{80DD32D5-408E-4A8D-9988-A29B58792556}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80DD32D5-408E-4A8D-9988-A29B58792556}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Jobs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -61,96 +61,21 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Xóa tài khoản User</t>
-  </si>
-  <si>
-    <t>Nhập thông tin giao hàng</t>
-  </si>
-  <si>
     <t>Xem thức uống</t>
   </si>
   <si>
-    <t>Thêm thông tin thức uống</t>
-  </si>
-  <si>
-    <t>Xóa thông tin thức uống</t>
-  </si>
-  <si>
-    <t>Sửa thông tin thức uống</t>
-  </si>
-  <si>
     <t>Đánh giá thức uống</t>
   </si>
   <si>
     <t>Xóa đơn hàng</t>
   </si>
   <si>
-    <t>Xem lịch sử đơn hàng user</t>
-  </si>
-  <si>
     <t>Xem lịch sử đơn hàng</t>
   </si>
   <si>
-    <t>Thêm thông tin thẻ tín dụng</t>
-  </si>
-  <si>
-    <t>Chọn hình thức thanh toán</t>
-  </si>
-  <si>
     <t>Xem giỏ hàng</t>
   </si>
   <si>
-    <t>Cho phép admin đăng nhập bằng tài khoản Admin định sẵn</t>
-  </si>
-  <si>
-    <t>Cho phép user đăng nhập bằng tài khoản User định sẵn</t>
-  </si>
-  <si>
-    <t>Cho phép user đăng ký bằng tài khoản User định sẵn</t>
-  </si>
-  <si>
-    <t>Cho phép admin xóa tài khoản của người dùng</t>
-  </si>
-  <si>
-    <t>Cho phép admin thêm thông tin thức uống</t>
-  </si>
-  <si>
-    <t>Cho phép admin xóa thông tin thức uống</t>
-  </si>
-  <si>
-    <t>Cho phép admin sửa thông tin thức uống</t>
-  </si>
-  <si>
-    <t>Cho phép admin xóa đơn hàng</t>
-  </si>
-  <si>
-    <t>Cho phép admin xem lịch sử đơn hàng user</t>
-  </si>
-  <si>
-    <t>Cho phép user nhập thông tin giao hàng</t>
-  </si>
-  <si>
-    <t>Cho phép user chọn thức uống</t>
-  </si>
-  <si>
-    <t>Cho phép user xem thức uống</t>
-  </si>
-  <si>
-    <t>Cho phép user chọn hình thức thanh toán</t>
-  </si>
-  <si>
-    <t>Cho phép user xem giỏ hàng của bản thân</t>
-  </si>
-  <si>
-    <t>Cho phép user thêm thông tin thẻ tín dụng của bản thân</t>
-  </si>
-  <si>
-    <t>Cho phép user xem lịch sử đơn hàng của bản thân</t>
-  </si>
-  <si>
-    <t>Cho phép user đánh giá thức của người dùng trên thức uống</t>
-  </si>
-  <si>
     <t>Basic Jobs ID</t>
   </si>
   <si>
@@ -241,15 +166,6 @@
     <t>Liên kết database lưu dữ liệu</t>
   </si>
   <si>
-    <t>Xem đơn hàng chưa giao</t>
-  </si>
-  <si>
-    <t>Cho phép admin xem đơn hàng chưa giao</t>
-  </si>
-  <si>
-    <t>Cho phép user xác nhận đơn của bản thân</t>
-  </si>
-  <si>
     <t>Tạo của số xem đơn hàng chưa giao</t>
   </si>
   <si>
@@ -263,6 +179,84 @@
   </si>
   <si>
     <t>Thêm thức uống vào giỏ</t>
+  </si>
+  <si>
+    <t>Cho phép đăng nhập vào tài khoản có sẵn</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin User</t>
+  </si>
+  <si>
+    <t>Cho phép admin xóa hoặc reset mật khẩu tài khoản người dùng</t>
+  </si>
+  <si>
+    <t>Quản lý sản phẩm</t>
+  </si>
+  <si>
+    <t>Thêm, xóa, sửa thông tin sản phẩm</t>
+  </si>
+  <si>
+    <t>Quản lý danh mục</t>
+  </si>
+  <si>
+    <t>Thêm, xóa, sửa các danh mục sản phẩm</t>
+  </si>
+  <si>
+    <t>Xem thống kê</t>
+  </si>
+  <si>
+    <t>Xem và đổi trạng thái ship của các đơn hàng chưa giao</t>
+  </si>
+  <si>
+    <t>Quản lý đơn hàng chưa giao</t>
+  </si>
+  <si>
+    <t>Ban hành tài khoản nhân viên</t>
+  </si>
+  <si>
+    <t>Tạo tài khoản với phân quyền nhân viên</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Đổi thông tin của tài khoản cá nhân</t>
+  </si>
+  <si>
+    <t>Đăng ký tài khoản mới nếu chưa có</t>
+  </si>
+  <si>
+    <t>Đặt hàng đã có trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>Chọn và thêm thức uống vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>Xóa các đơn hàng nghi vấn bom, đặt nhầm</t>
+  </si>
+  <si>
+    <t>Hiển thị các thống kê gồm doanh thu theo tháng, theo năm, vv</t>
+  </si>
+  <si>
+    <t>Đánh giá các thức uống đã mua</t>
+  </si>
+  <si>
+    <t>Xem thức uống và thông tin trong danh mục sản phẩm của cửa hàng</t>
+  </si>
+  <si>
+    <t>Xem được giỏ hàng và các mặt hàng đã thêm vào</t>
+  </si>
+  <si>
+    <t>Xem lịch sử các đơn hàng đã mua trước đây của bản thân</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Cho phép đăng xuất khỏi tài khoản đang đăng nhập</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
   </si>
 </sst>
 </file>
@@ -334,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91A7117C-93D8-4709-8EE7-B08ECDDAA76E}" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D20" xr:uid="{91A7117C-93D8-4709-8EE7-B08ECDDAA76E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91A7117C-93D8-4709-8EE7-B08ECDDAA76E}" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D25" xr:uid="{91A7117C-93D8-4709-8EE7-B08ECDDAA76E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{860EEE4C-A1AD-4FD7-B11B-0FEAB61CD593}" name="ID"/>
     <tableColumn id="2" xr3:uid="{5248838F-AF28-43B8-9527-3DB306F3BD67}" name="Tính năng"/>
@@ -643,21 +637,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A54548-1764-402D-9134-0FD67590CD37}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,270 +665,340 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -953,28 +1017,28 @@
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -983,13 +1047,13 @@
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(B2, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin đăng nhập bằng tài khoản Admin định sẵn</v>
+        <v>Cho phép admin xóa hoặc reset mật khẩu tài khoản người dùng</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -998,13 +1062,13 @@
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(B3, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin đăng nhập bằng tài khoản Admin định sẵn</v>
+        <v>Cho phép admin xóa hoặc reset mật khẩu tài khoản người dùng</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1013,13 +1077,13 @@
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(B4, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin đăng nhập bằng tài khoản Admin định sẵn</v>
+        <v>Cho phép admin xóa hoặc reset mật khẩu tài khoản người dùng</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1028,13 +1092,13 @@
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(B5, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin đăng nhập bằng tài khoản Admin định sẵn</v>
+        <v>Cho phép admin xóa hoặc reset mật khẩu tài khoản người dùng</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1043,13 +1107,13 @@
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(B6, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa tài khoản của người dùng</v>
+        <v>Thêm, xóa, sửa thông tin sản phẩm</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1058,13 +1122,13 @@
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(B7, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa tài khoản của người dùng</v>
+        <v>Thêm, xóa, sửa thông tin sản phẩm</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1073,13 +1137,13 @@
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP(B8, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa tài khoản của người dùng</v>
+        <v>Thêm, xóa, sửa thông tin sản phẩm</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1088,13 +1152,13 @@
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(B9, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa tài khoản của người dùng</v>
+        <v>Thêm, xóa, sửa thông tin sản phẩm</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1103,13 +1167,13 @@
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP(B10, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa tài khoản của người dùng</v>
+        <v>Thêm, xóa, sửa thông tin sản phẩm</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1118,13 +1182,13 @@
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(B11, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin thêm thông tin thức uống</v>
+        <v>Thêm, xóa, sửa các danh mục sản phẩm</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1133,13 +1197,13 @@
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP(B12, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin thêm thông tin thức uống</v>
+        <v>Thêm, xóa, sửa các danh mục sản phẩm</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1148,13 +1212,13 @@
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP(B13, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin thêm thông tin thức uống</v>
+        <v>Thêm, xóa, sửa các danh mục sản phẩm</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1163,13 +1227,13 @@
       </c>
       <c r="C14" t="str">
         <f>VLOOKUP(B14, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin thêm thông tin thức uống</v>
+        <v>Thêm, xóa, sửa các danh mục sản phẩm</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1178,13 +1242,13 @@
       </c>
       <c r="C15" t="str">
         <f>VLOOKUP(B15, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa thông tin thức uống</v>
+        <v>Hiển thị các thống kê gồm doanh thu theo tháng, theo năm, vv</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1193,13 +1257,13 @@
       </c>
       <c r="C16" t="str">
         <f>VLOOKUP(B16, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa thông tin thức uống</v>
+        <v>Hiển thị các thống kê gồm doanh thu theo tháng, theo năm, vv</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1208,13 +1272,13 @@
       </c>
       <c r="C17" t="str">
         <f>VLOOKUP(B17, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa thông tin thức uống</v>
+        <v>Hiển thị các thống kê gồm doanh thu theo tháng, theo năm, vv</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1223,13 +1287,13 @@
       </c>
       <c r="C18" t="str">
         <f>VLOOKUP(B18, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin sửa thông tin thức uống</v>
+        <v>Xem và đổi trạng thái ship của các đơn hàng chưa giao</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1238,13 +1302,13 @@
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP(B19, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin sửa thông tin thức uống</v>
+        <v>Xem và đổi trạng thái ship của các đơn hàng chưa giao</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1253,13 +1317,13 @@
       </c>
       <c r="C20" t="str">
         <f>VLOOKUP(B20, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin sửa thông tin thức uống</v>
+        <v>Xem và đổi trạng thái ship của các đơn hàng chưa giao</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1268,13 +1332,13 @@
       </c>
       <c r="C21" t="str">
         <f>VLOOKUP(B21, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa đơn hàng</v>
+        <v>Xóa các đơn hàng nghi vấn bom, đặt nhầm</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1283,13 +1347,13 @@
       </c>
       <c r="C22" t="str">
         <f>VLOOKUP(B22, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa đơn hàng</v>
+        <v>Xóa các đơn hàng nghi vấn bom, đặt nhầm</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1298,13 +1362,13 @@
       </c>
       <c r="C23" t="str">
         <f>VLOOKUP(B23, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa đơn hàng</v>
+        <v>Xóa các đơn hàng nghi vấn bom, đặt nhầm</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1313,13 +1377,13 @@
       </c>
       <c r="C24" t="str">
         <f>VLOOKUP(B24, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xóa đơn hàng</v>
+        <v>Xóa các đơn hàng nghi vấn bom, đặt nhầm</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1328,13 +1392,13 @@
       </c>
       <c r="C25" t="str">
         <f>VLOOKUP(B25, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem lịch sử đơn hàng user</v>
+        <v>Tạo tài khoản với phân quyền nhân viên</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1343,13 +1407,13 @@
       </c>
       <c r="C26" t="str">
         <f>VLOOKUP(B26, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem lịch sử đơn hàng user</v>
+        <v>Tạo tài khoản với phân quyền nhân viên</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1358,13 +1422,13 @@
       </c>
       <c r="C27" t="str">
         <f>VLOOKUP(B27, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem lịch sử đơn hàng user</v>
+        <v>Tạo tài khoản với phân quyền nhân viên</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1373,13 +1437,13 @@
       </c>
       <c r="C28" t="str">
         <f>VLOOKUP(B28, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem đơn hàng chưa giao</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1388,13 +1452,13 @@
       </c>
       <c r="C29" t="str">
         <f>VLOOKUP(B29, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem đơn hàng chưa giao</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1403,13 +1467,13 @@
       </c>
       <c r="C30" t="str">
         <f>VLOOKUP(B30, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem đơn hàng chưa giao</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1418,13 +1482,13 @@
       </c>
       <c r="C31" t="str">
         <f>VLOOKUP(B31, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép admin xem đơn hàng chưa giao</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1433,13 +1497,13 @@
       </c>
       <c r="C32" t="str">
         <f>VLOOKUP(B32, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user đăng nhập bằng tài khoản User định sẵn</v>
+        <v>Đổi thông tin của tài khoản cá nhân</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1448,13 +1512,13 @@
       </c>
       <c r="C33" t="str">
         <f>VLOOKUP(B33, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user đăng ký bằng tài khoản User định sẵn</v>
+        <v>Cho phép đăng xuất khỏi tài khoản đang đăng nhập</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1463,13 +1527,13 @@
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP(B34, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user đăng ký bằng tài khoản User định sẵn</v>
+        <v>Cho phép đăng xuất khỏi tài khoản đang đăng nhập</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1478,13 +1542,13 @@
       </c>
       <c r="C35" t="str">
         <f>VLOOKUP(B35, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user đăng ký bằng tài khoản User định sẵn</v>
+        <v>Cho phép đăng xuất khỏi tài khoản đang đăng nhập</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1493,13 +1557,13 @@
       </c>
       <c r="C36" t="str">
         <f>VLOOKUP(B36, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user nhập thông tin giao hàng</v>
+        <v>Xem và đổi trạng thái ship của các đơn hàng chưa giao</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1508,13 +1572,13 @@
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP(B37, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user nhập thông tin giao hàng</v>
+        <v>Xem và đổi trạng thái ship của các đơn hàng chưa giao</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1523,13 +1587,13 @@
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP(B38, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user xác nhận đơn của bản thân</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1538,13 +1602,13 @@
       </c>
       <c r="C39" t="str">
         <f>VLOOKUP(B39, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user xác nhận đơn của bản thân</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1553,13 +1617,13 @@
       </c>
       <c r="C40" t="str">
         <f>VLOOKUP(B40, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user xác nhận đơn của bản thân</v>
+        <v>Cho phép đăng nhập vào tài khoản có sẵn</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1568,10 +1632,10 @@
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP(B41, Table1[#All], 4, FALSE)</f>
-        <v>Cho phép user chọn thức uống</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>Đổi thông tin của tài khoản cá nhân</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1580,7 +1644,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1589,7 +1653,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1598,7 +1662,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1607,7 +1671,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1616,7 +1680,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1625,7 +1689,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1634,7 +1698,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1643,7 +1707,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>

</xml_diff>